<commit_message>
added special register standards
</commit_message>
<xml_diff>
--- a/documents/new-instructions.xlsx
+++ b/documents/new-instructions.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="91">
   <si>
     <t>Instruction</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Register</t>
   </si>
   <si>
-    <t>Purpose</t>
-  </si>
-  <si>
     <t>beq $rd, $rs, N</t>
   </si>
   <si>
@@ -87,6 +84,225 @@
   </si>
   <si>
     <t>Note: capacitive sensors read one value every 100,000 cycles</t>
+  </si>
+  <si>
+    <t>$r0</t>
+  </si>
+  <si>
+    <t>$r1</t>
+  </si>
+  <si>
+    <t>$r2</t>
+  </si>
+  <si>
+    <t>$r3</t>
+  </si>
+  <si>
+    <t>$r4</t>
+  </si>
+  <si>
+    <t>$r5</t>
+  </si>
+  <si>
+    <t>$r6</t>
+  </si>
+  <si>
+    <t>$r7</t>
+  </si>
+  <si>
+    <t>$r8</t>
+  </si>
+  <si>
+    <t>$r9</t>
+  </si>
+  <si>
+    <t>$r10</t>
+  </si>
+  <si>
+    <t>$r11</t>
+  </si>
+  <si>
+    <t>$r12</t>
+  </si>
+  <si>
+    <t>$r13</t>
+  </si>
+  <si>
+    <t>$r14</t>
+  </si>
+  <si>
+    <t>$r15</t>
+  </si>
+  <si>
+    <t>$r16</t>
+  </si>
+  <si>
+    <t>$r17</t>
+  </si>
+  <si>
+    <t>$r18</t>
+  </si>
+  <si>
+    <t>$r19</t>
+  </si>
+  <si>
+    <t>$r20</t>
+  </si>
+  <si>
+    <t>$r21</t>
+  </si>
+  <si>
+    <t>$r22</t>
+  </si>
+  <si>
+    <t>$r23</t>
+  </si>
+  <si>
+    <t>$r24</t>
+  </si>
+  <si>
+    <t>$r25</t>
+  </si>
+  <si>
+    <t>$r26</t>
+  </si>
+  <si>
+    <t>$r27</t>
+  </si>
+  <si>
+    <t>$r28</t>
+  </si>
+  <si>
+    <t>$r30</t>
+  </si>
+  <si>
+    <t>$r31</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>zero</t>
+  </si>
+  <si>
+    <t>function return value</t>
+  </si>
+  <si>
+    <t>function argument</t>
+  </si>
+  <si>
+    <t>stack pointer (starts at 0)</t>
+  </si>
+  <si>
+    <t>temporary variables (need not preserve)</t>
+  </si>
+  <si>
+    <t>function variables (preserve before calling)</t>
+  </si>
+  <si>
+    <t>Alias</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>$v0</t>
+  </si>
+  <si>
+    <t>$v1</t>
+  </si>
+  <si>
+    <t>$a0</t>
+  </si>
+  <si>
+    <t>$a1</t>
+  </si>
+  <si>
+    <t>$a2</t>
+  </si>
+  <si>
+    <t>$a3</t>
+  </si>
+  <si>
+    <t>$t0</t>
+  </si>
+  <si>
+    <t>$t1</t>
+  </si>
+  <si>
+    <t>$t2</t>
+  </si>
+  <si>
+    <t>$t3</t>
+  </si>
+  <si>
+    <t>$t4</t>
+  </si>
+  <si>
+    <t>$t5</t>
+  </si>
+  <si>
+    <t>$t6</t>
+  </si>
+  <si>
+    <t>$t7</t>
+  </si>
+  <si>
+    <t>$t8</t>
+  </si>
+  <si>
+    <t>$t9</t>
+  </si>
+  <si>
+    <t>$t10</t>
+  </si>
+  <si>
+    <t>$t11</t>
+  </si>
+  <si>
+    <t>$t12</t>
+  </si>
+  <si>
+    <t>$s0</t>
+  </si>
+  <si>
+    <t>$s1</t>
+  </si>
+  <si>
+    <t>$s2</t>
+  </si>
+  <si>
+    <t>$s3</t>
+  </si>
+  <si>
+    <t>$s4</t>
+  </si>
+  <si>
+    <t>$s5</t>
+  </si>
+  <si>
+    <t>$s6</t>
+  </si>
+  <si>
+    <t>$s7</t>
+  </si>
+  <si>
+    <t>$sp</t>
+  </si>
+  <si>
+    <t>$ra</t>
+  </si>
+  <si>
+    <t>$rm</t>
+  </si>
+  <si>
+    <t>$rstatus</t>
+  </si>
+  <si>
+    <t>exception status</t>
+  </si>
+  <si>
+    <t>return address</t>
   </si>
 </sst>
 </file>
@@ -125,12 +341,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB4C7E7"/>
-        <bgColor rgb="FFB4C6E7"/>
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -139,90 +355,34 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
+      <left/>
       <right/>
       <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
+        <color theme="2" tint="-0.249977111117893"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color theme="2" tint="-0.249977111117893"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
-        <color auto="1"/>
+        <color theme="2" tint="-0.249977111117893"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
+      <top style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color theme="2" tint="-0.249977111117893"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -231,41 +391,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -615,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -626,91 +764,432 @@
     <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="8.83203125" style="2"/>
     <col min="4" max="4" width="25.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="33" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" customWidth="1"/>
+    <col min="10" max="10" width="26.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1"/>
+      <c r="J1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="D2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="F2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="F6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="1"/>
+      <c r="F8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F12" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F13" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F14" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F15" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F16" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="F17" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="F18" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D19" s="4"/>
+      <c r="F19" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="F20" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="F21" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="F22" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="F23" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="F24" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="F25" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="F26" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="F27" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="F28" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="F29" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="F30" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="F31" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G31" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="H31" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="1"/>
+    </row>
+    <row r="32" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="F32" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="F33" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>90</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>